<commit_message>
Added some example data and information on how to use the package in the README
</commit_message>
<xml_diff>
--- a/inst/extdata/brightness_update210301.xlsx
+++ b/inst/extdata/brightness_update210301.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Ongoing\PanelDesignR\inst\extdata\Catalogues\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_repos\CytoBright\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13848"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="166">
   <si>
     <t>Fluorochrome</t>
   </si>
@@ -530,6 +530,9 @@
   </si>
   <si>
     <t>Brightness BD+BL+TF+FF+PN</t>
+  </si>
+  <si>
+    <t>Maximum value</t>
   </si>
 </sst>
 </file>
@@ -917,7 +920,7 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1501,7 +1504,7 @@
         <v>5</v>
       </c>
       <c r="I22">
-        <f>((D22*4)+(G22*5))/9</f>
+        <f t="shared" ref="I22:I28" si="1">((D22*4)+(G22*5))/9</f>
         <v>4.5555555555555554</v>
       </c>
       <c r="J22">
@@ -1526,7 +1529,7 @@
         <v>5</v>
       </c>
       <c r="I23">
-        <f>((D23*4)+(G23*5))/9</f>
+        <f t="shared" si="1"/>
         <v>4.5555555555555554</v>
       </c>
       <c r="J23">
@@ -1551,7 +1554,7 @@
         <v>3</v>
       </c>
       <c r="I24">
-        <f>((D24*4)+(G24*5))/9</f>
+        <f t="shared" si="1"/>
         <v>3.4444444444444446</v>
       </c>
       <c r="J24">
@@ -1576,7 +1579,7 @@
         <v>5</v>
       </c>
       <c r="I25">
-        <f>((D25*4)+(G25*5))/9</f>
+        <f t="shared" si="1"/>
         <v>4.5555555555555554</v>
       </c>
       <c r="J25">
@@ -1601,11 +1604,11 @@
         <v>2</v>
       </c>
       <c r="I26">
-        <f>((D26*4)+(G26*5))/9</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26:J43" si="1">ROUND(I26,0)</f>
+        <f t="shared" ref="J26:J43" si="2">ROUND(I26,0)</f>
         <v>2</v>
       </c>
     </row>
@@ -1626,11 +1629,11 @@
         <v>2</v>
       </c>
       <c r="I27">
-        <f>((D27*4)+(G27*5))/9</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -1651,11 +1654,11 @@
         <v>4</v>
       </c>
       <c r="I28">
-        <f>((D28*4)+(G28*5))/9</f>
+        <f t="shared" si="1"/>
         <v>3.5555555555555554</v>
       </c>
       <c r="J28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -1677,7 +1680,7 @@
         <v>3</v>
       </c>
       <c r="J29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -1702,7 +1705,7 @@
         <v>3.5555555555555554</v>
       </c>
       <c r="J30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -1727,7 +1730,7 @@
         <v>3.5555555555555554</v>
       </c>
       <c r="J31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -1752,7 +1755,7 @@
         <v>1</v>
       </c>
       <c r="J32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1780,7 +1783,7 @@
         <v>4.3571428571428568</v>
       </c>
       <c r="J33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -1805,7 +1808,7 @@
         <v>3.5555555555555554</v>
       </c>
       <c r="J34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -1833,7 +1836,7 @@
         <v>2</v>
       </c>
       <c r="J35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -1861,7 +1864,7 @@
         <v>2</v>
       </c>
       <c r="J36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -1889,7 +1892,7 @@
         <v>3.3571428571428572</v>
       </c>
       <c r="J37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -1917,7 +1920,7 @@
         <v>3.6428571428571428</v>
       </c>
       <c r="J38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -1945,7 +1948,7 @@
         <v>4</v>
       </c>
       <c r="J39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -1973,7 +1976,7 @@
         <v>3.0714285714285716</v>
       </c>
       <c r="J40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -1998,7 +2001,7 @@
         <v>3</v>
       </c>
       <c r="J41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -2023,7 +2026,7 @@
         <v>3</v>
       </c>
       <c r="J42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -2045,7 +2048,7 @@
         <v>4</v>
       </c>
       <c r="J43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -2083,7 +2086,7 @@
         <v>4</v>
       </c>
       <c r="J46">
-        <f t="shared" ref="J46:J61" si="2">ROUND(I46,0)</f>
+        <f t="shared" ref="J46:J61" si="3">ROUND(I46,0)</f>
         <v>4</v>
       </c>
     </row>
@@ -2130,7 +2133,7 @@
         <v>2</v>
       </c>
       <c r="J49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -2152,7 +2155,7 @@
         <v>1</v>
       </c>
       <c r="J50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2177,7 +2180,7 @@
         <v>4</v>
       </c>
       <c r="J51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -2233,7 +2236,7 @@
         <v>1.7916666666666667</v>
       </c>
       <c r="J54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -2269,7 +2272,7 @@
         <v>3</v>
       </c>
       <c r="J56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -2285,7 +2288,7 @@
         <v>1</v>
       </c>
       <c r="J57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2306,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="J58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2322,7 +2325,7 @@
         <v>1</v>
       </c>
       <c r="J59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2338,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="J60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2359,7 +2362,7 @@
         <v>1</v>
       </c>
       <c r="J61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2412,7 +2415,7 @@
         <v>5</v>
       </c>
       <c r="J64">
-        <f t="shared" ref="J64:J79" si="3">ROUND(I64,0)</f>
+        <f t="shared" ref="J64:J79" si="4">ROUND(I64,0)</f>
         <v>5</v>
       </c>
     </row>
@@ -2428,7 +2431,7 @@
         <v>4</v>
       </c>
       <c r="J65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
@@ -2444,7 +2447,7 @@
         <v>3</v>
       </c>
       <c r="J66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -2465,7 +2468,7 @@
         <v>2</v>
       </c>
       <c r="J67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -2486,7 +2489,7 @@
         <v>3</v>
       </c>
       <c r="J68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -2507,7 +2510,7 @@
         <v>2</v>
       </c>
       <c r="J69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -2523,7 +2526,7 @@
         <v>5</v>
       </c>
       <c r="J70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -2539,7 +2542,7 @@
         <v>5</v>
       </c>
       <c r="J71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -2555,7 +2558,7 @@
         <v>3</v>
       </c>
       <c r="J72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -2586,7 +2589,7 @@
         <v>1.5263157894736843</v>
       </c>
       <c r="J73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -2611,7 +2614,7 @@
         <v>1</v>
       </c>
       <c r="J74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -2645,7 +2648,7 @@
         <v>4.666666666666667</v>
       </c>
       <c r="J75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -2672,7 +2675,7 @@
         <v>2</v>
       </c>
       <c r="J77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -2697,7 +2700,7 @@
         <v>4</v>
       </c>
       <c r="J78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
@@ -2728,7 +2731,7 @@
         <v>4.7894736842105265</v>
       </c>
       <c r="J79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -2815,7 +2818,7 @@
         <v>5</v>
       </c>
       <c r="J82">
-        <f t="shared" ref="J82:J101" si="4">ROUND(I82,0)</f>
+        <f t="shared" ref="J82:J101" si="5">ROUND(I82,0)</f>
         <v>5</v>
       </c>
     </row>
@@ -2840,7 +2843,7 @@
         <v>3</v>
       </c>
       <c r="J83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -2856,7 +2859,7 @@
         <v>4</v>
       </c>
       <c r="J84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
@@ -2877,7 +2880,7 @@
         <v>5</v>
       </c>
       <c r="J85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -2899,7 +2902,7 @@
         <v>4</v>
       </c>
       <c r="J86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
@@ -2915,7 +2918,7 @@
         <v>4</v>
       </c>
       <c r="J87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
@@ -2938,7 +2941,7 @@
         <v>1</v>
       </c>
       <c r="J88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -2972,7 +2975,7 @@
         <v>2</v>
       </c>
       <c r="J89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3000,7 +3003,7 @@
         <v>4</v>
       </c>
       <c r="J90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
@@ -3021,7 +3024,7 @@
         <v>2.5</v>
       </c>
       <c r="J91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -3042,7 +3045,7 @@
         <v>5</v>
       </c>
       <c r="J92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -3059,7 +3062,7 @@
         <v>5</v>
       </c>
       <c r="J93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -3097,7 +3100,7 @@
         <v>5</v>
       </c>
       <c r="J95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -3122,7 +3125,7 @@
         <v>5</v>
       </c>
       <c r="J96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -3143,7 +3146,7 @@
         <v>5</v>
       </c>
       <c r="J97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -3159,7 +3162,7 @@
         <v>5</v>
       </c>
       <c r="J98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -3180,7 +3183,7 @@
         <v>3</v>
       </c>
       <c r="J99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -3205,7 +3208,7 @@
         <v>4.5</v>
       </c>
       <c r="J100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -3230,7 +3233,7 @@
         <v>5</v>
       </c>
       <c r="J101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -3322,7 +3325,7 @@
         <v>1</v>
       </c>
       <c r="J105">
-        <f t="shared" ref="J105:J114" si="5">ROUND(I105,0)</f>
+        <f t="shared" ref="J105:J114" si="6">ROUND(I105,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3343,7 +3346,7 @@
         <v>3</v>
       </c>
       <c r="J106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
@@ -3360,7 +3363,7 @@
         <v>1</v>
       </c>
       <c r="J107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3377,7 +3380,7 @@
         <v>2</v>
       </c>
       <c r="J108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
     </row>
@@ -3413,7 +3416,7 @@
         <v>1.5555555555555556</v>
       </c>
       <c r="J110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
     </row>
@@ -3438,7 +3441,7 @@
         <v>1.5555555555555556</v>
       </c>
       <c r="J111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
     </row>
@@ -3454,7 +3457,7 @@
         <v>4</v>
       </c>
       <c r="J112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
@@ -3470,7 +3473,7 @@
         <v>5</v>
       </c>
       <c r="J113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
     </row>
@@ -3486,7 +3489,7 @@
         <v>4</v>
       </c>
       <c r="J114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
@@ -3502,6 +3505,9 @@
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="C117" t="s">
+        <v>165</v>
+      </c>
       <c r="D117" s="8">
         <v>4</v>
       </c>

</xml_diff>